<commit_message>
sprint2 tasks and user stories finished along with pair programming task
</commit_message>
<xml_diff>
--- a/Team05.xlsx
+++ b/Team05.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="268">
   <si>
     <t>This document was exported from Numbers. Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -777,6 +777,36 @@
   </si>
   <si>
     <t>Perform validation to see whether marriage after the age of 14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check and store birth </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check and store marital status date of parents </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare both </t>
+  </si>
+  <si>
+    <t>T09.01</t>
+  </si>
+  <si>
+    <t>T09.02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check and store death of mother </t>
+  </si>
+  <si>
+    <t>T09.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check and store death of Father </t>
+  </si>
+  <si>
+    <t>T09.04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare birth with smallest date of death of parents </t>
   </si>
   <si>
     <t>T011.01</t>
@@ -3216,7 +3246,7 @@
     </row>
     <row r="21">
       <c r="B21" t="s" s="3">
-        <v>249</v>
+        <v>259</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -3227,7 +3257,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s" s="5">
-        <v>249</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -11845,7 +11875,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J47"/>
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -12175,11 +12205,11 @@
       <c r="J18" s="28"/>
     </row>
     <row r="19" ht="15.25" customHeight="1">
-      <c r="A19" t="s" s="38">
-        <v>55</v>
-      </c>
-      <c r="B19" t="s" s="38">
-        <v>189</v>
+      <c r="A19" t="s" s="33">
+        <v>61</v>
+      </c>
+      <c r="B19" t="s" s="33">
+        <v>62</v>
       </c>
       <c r="C19" t="s" s="33">
         <v>31</v>
@@ -12210,10 +12240,10 @@
     </row>
     <row r="21" ht="15.25" customHeight="1">
       <c r="A21" t="s" s="33">
-        <v>190</v>
+        <v>210</v>
       </c>
       <c r="B21" t="s" s="35">
-        <v>182</v>
+        <v>240</v>
       </c>
       <c r="C21" t="s" s="33">
         <v>31</v>
@@ -12226,12 +12256,12 @@
       <c r="I21" s="28"/>
       <c r="J21" s="28"/>
     </row>
-    <row r="22" ht="15.25" customHeight="1">
+    <row r="22" ht="15.35" customHeight="1">
       <c r="A22" t="s" s="33">
-        <v>191</v>
+        <v>211</v>
       </c>
       <c r="B22" t="s" s="35">
-        <v>192</v>
+        <v>241</v>
       </c>
       <c r="C22" t="s" s="33">
         <v>31</v>
@@ -12246,10 +12276,10 @@
     </row>
     <row r="23" ht="15.25" customHeight="1">
       <c r="A23" t="s" s="33">
-        <v>193</v>
+        <v>213</v>
       </c>
       <c r="B23" t="s" s="35">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="C23" t="s" s="33">
         <v>31</v>
@@ -12263,15 +12293,9 @@
       <c r="J23" s="28"/>
     </row>
     <row r="24" ht="15.25" customHeight="1">
-      <c r="A24" t="s" s="33">
-        <v>194</v>
-      </c>
-      <c r="B24" t="s" s="35">
-        <v>195</v>
-      </c>
-      <c r="C24" t="s" s="33">
-        <v>31</v>
-      </c>
+      <c r="A24" s="28"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
       <c r="F24" s="28"/>
@@ -12280,28 +12304,32 @@
       <c r="I24" s="28"/>
       <c r="J24" s="28"/>
     </row>
-    <row r="25" ht="16" customHeight="1">
+    <row r="25" ht="15.25" customHeight="1">
       <c r="A25" t="s" s="33">
-        <v>196</v>
-      </c>
-      <c r="B25" t="s" s="35">
-        <v>197</v>
+        <v>64</v>
+      </c>
+      <c r="B25" t="s" s="33">
+        <v>65</v>
       </c>
       <c r="C25" t="s" s="33">
         <v>31</v>
       </c>
       <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
+      <c r="E25" s="42">
+        <v>22</v>
+      </c>
+      <c r="F25" s="42">
+        <v>80</v>
+      </c>
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
       <c r="J25" s="28"/>
     </row>
     <row r="26" ht="15.25" customHeight="1">
-      <c r="A26" s="28"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
+      <c r="A26" s="43"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
       <c r="F26" s="28"/>
@@ -12311,31 +12339,33 @@
       <c r="J26" s="28"/>
     </row>
     <row r="27" ht="15.25" customHeight="1">
-      <c r="A27" t="s" s="38">
-        <v>58</v>
-      </c>
-      <c r="B27" t="s" s="33">
-        <v>59</v>
+      <c r="A27" t="s" s="33">
+        <v>243</v>
+      </c>
+      <c r="B27" t="s" s="35">
+        <v>184</v>
       </c>
       <c r="C27" t="s" s="33">
         <v>31</v>
       </c>
       <c r="D27" s="28"/>
-      <c r="E27" s="42">
-        <v>22</v>
-      </c>
-      <c r="F27" s="42">
-        <v>80</v>
-      </c>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="28"/>
       <c r="J27" s="28"/>
     </row>
     <row r="28" ht="15.25" customHeight="1">
-      <c r="A28" s="43"/>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
+      <c r="A28" t="s" s="33">
+        <v>244</v>
+      </c>
+      <c r="B28" t="s" s="35">
+        <v>245</v>
+      </c>
+      <c r="C28" t="s" s="33">
+        <v>31</v>
+      </c>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
       <c r="F28" s="28"/>
@@ -12344,12 +12374,12 @@
       <c r="I28" s="28"/>
       <c r="J28" s="28"/>
     </row>
-    <row r="29" ht="15.25" customHeight="1">
+    <row r="29" ht="16" customHeight="1">
       <c r="A29" t="s" s="33">
-        <v>198</v>
+        <v>246</v>
       </c>
       <c r="B29" t="s" s="35">
-        <v>184</v>
+        <v>247</v>
       </c>
       <c r="C29" t="s" s="33">
         <v>31</v>
@@ -12364,10 +12394,10 @@
     </row>
     <row r="30" ht="15.25" customHeight="1">
       <c r="A30" t="s" s="33">
-        <v>199</v>
+        <v>248</v>
       </c>
       <c r="B30" t="s" s="35">
-        <v>178</v>
+        <v>249</v>
       </c>
       <c r="C30" t="s" s="33">
         <v>31</v>
@@ -12380,16 +12410,10 @@
       <c r="I30" s="28"/>
       <c r="J30" s="28"/>
     </row>
-    <row r="31" ht="16" customHeight="1">
-      <c r="A31" t="s" s="33">
-        <v>200</v>
-      </c>
-      <c r="B31" t="s" s="35">
-        <v>201</v>
-      </c>
-      <c r="C31" t="s" s="33">
-        <v>31</v>
-      </c>
+    <row r="31" ht="15.25" customHeight="1">
+      <c r="A31" s="28"/>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
       <c r="F31" s="28"/>
@@ -12399,21 +12423,31 @@
       <c r="J31" s="28"/>
     </row>
     <row r="32" ht="15.25" customHeight="1">
-      <c r="A32" s="28"/>
-      <c r="B32" s="28"/>
-      <c r="C32" s="28"/>
+      <c r="A32" t="s" s="38">
+        <v>70</v>
+      </c>
+      <c r="B32" t="s" s="33">
+        <v>71</v>
+      </c>
+      <c r="C32" t="s" s="33">
+        <v>21</v>
+      </c>
       <c r="D32" s="28"/>
-      <c r="E32" s="28"/>
-      <c r="F32" s="28"/>
+      <c r="E32" s="42">
+        <v>20</v>
+      </c>
+      <c r="F32" s="42">
+        <v>120</v>
+      </c>
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
       <c r="J32" s="28"/>
     </row>
     <row r="33" ht="15.25" customHeight="1">
-      <c r="A33" s="28"/>
-      <c r="B33" s="28"/>
-      <c r="C33" s="28"/>
+      <c r="A33" s="43"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="28"/>
       <c r="E33" s="28"/>
       <c r="F33" s="28"/>
@@ -12423,45 +12457,47 @@
       <c r="J33" s="28"/>
     </row>
     <row r="34" ht="15.25" customHeight="1">
-      <c r="A34" t="s" s="38">
-        <v>70</v>
-      </c>
-      <c r="B34" t="s" s="33">
-        <v>71</v>
+      <c r="A34" t="s" s="33">
+        <v>250</v>
+      </c>
+      <c r="B34" t="s" s="35">
+        <v>182</v>
       </c>
       <c r="C34" t="s" s="33">
         <v>21</v>
       </c>
-      <c r="D34" s="28"/>
-      <c r="E34" s="42">
-        <v>20</v>
-      </c>
-      <c r="F34" s="42">
-        <v>120</v>
-      </c>
+      <c r="D34" s="39"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28"/>
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
-      <c r="I34" s="28"/>
-      <c r="J34" s="28"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
     </row>
     <row r="35" ht="15.25" customHeight="1">
-      <c r="A35" s="43"/>
-      <c r="B35" s="43"/>
-      <c r="C35" s="43"/>
-      <c r="D35" s="28"/>
+      <c r="A35" t="s" s="33">
+        <v>250</v>
+      </c>
+      <c r="B35" t="s" s="35">
+        <v>192</v>
+      </c>
+      <c r="C35" t="s" s="33">
+        <v>21</v>
+      </c>
+      <c r="D35" s="39"/>
       <c r="E35" s="28"/>
       <c r="F35" s="28"/>
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
-      <c r="I35" s="28"/>
-      <c r="J35" s="28"/>
+      <c r="I35" s="39"/>
+      <c r="J35" s="39"/>
     </row>
     <row r="36" ht="15.25" customHeight="1">
       <c r="A36" t="s" s="33">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="B36" t="s" s="35">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c r="C36" t="s" s="33">
         <v>21</v>
@@ -12476,10 +12512,10 @@
     </row>
     <row r="37" ht="15.25" customHeight="1">
       <c r="A37" t="s" s="33">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="B37" t="s" s="35">
-        <v>192</v>
+        <v>251</v>
       </c>
       <c r="C37" t="s" s="33">
         <v>21</v>
@@ -12492,12 +12528,12 @@
       <c r="I37" s="39"/>
       <c r="J37" s="39"/>
     </row>
-    <row r="38" ht="15.25" customHeight="1">
+    <row r="38" ht="16" customHeight="1">
       <c r="A38" t="s" s="33">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="B38" t="s" s="35">
-        <v>206</v>
+        <v>252</v>
       </c>
       <c r="C38" t="s" s="33">
         <v>21</v>
@@ -12511,45 +12547,43 @@
       <c r="J38" s="39"/>
     </row>
     <row r="39" ht="15.25" customHeight="1">
-      <c r="A39" t="s" s="33">
-        <v>240</v>
-      </c>
-      <c r="B39" t="s" s="35">
-        <v>241</v>
-      </c>
-      <c r="C39" t="s" s="33">
-        <v>21</v>
-      </c>
-      <c r="D39" s="39"/>
+      <c r="A39" s="28"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28"/>
       <c r="E39" s="28"/>
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
-    </row>
-    <row r="40" ht="16" customHeight="1">
-      <c r="A40" t="s" s="33">
-        <v>240</v>
-      </c>
-      <c r="B40" t="s" s="35">
-        <v>242</v>
+      <c r="I39" s="28"/>
+      <c r="J39" s="28"/>
+    </row>
+    <row r="40" ht="15.25" customHeight="1">
+      <c r="A40" t="s" s="38">
+        <v>73</v>
+      </c>
+      <c r="B40" t="s" s="33">
+        <v>74</v>
       </c>
       <c r="C40" t="s" s="33">
         <v>21</v>
       </c>
       <c r="D40" s="39"/>
-      <c r="E40" s="28"/>
-      <c r="F40" s="28"/>
+      <c r="E40" s="42">
+        <v>18</v>
+      </c>
+      <c r="F40" s="42">
+        <v>110</v>
+      </c>
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
       <c r="I40" s="39"/>
       <c r="J40" s="39"/>
     </row>
     <row r="41" ht="15.25" customHeight="1">
-      <c r="A41" s="28"/>
-      <c r="B41" s="28"/>
-      <c r="C41" s="28"/>
+      <c r="A41" s="43"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="43"/>
       <c r="D41" s="28"/>
       <c r="E41" s="28"/>
       <c r="F41" s="28"/>
@@ -12559,45 +12593,47 @@
       <c r="J41" s="28"/>
     </row>
     <row r="42" ht="15.25" customHeight="1">
-      <c r="A42" t="s" s="38">
-        <v>73</v>
-      </c>
-      <c r="B42" t="s" s="33">
-        <v>74</v>
+      <c r="A42" t="s" s="33">
+        <v>253</v>
+      </c>
+      <c r="B42" t="s" s="35">
+        <v>184</v>
       </c>
       <c r="C42" t="s" s="33">
         <v>21</v>
       </c>
       <c r="D42" s="39"/>
-      <c r="E42" s="42">
-        <v>18</v>
-      </c>
-      <c r="F42" s="42">
-        <v>110</v>
-      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28"/>
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
       <c r="I42" s="39"/>
       <c r="J42" s="39"/>
     </row>
     <row r="43" ht="15.25" customHeight="1">
-      <c r="A43" s="43"/>
-      <c r="B43" s="43"/>
-      <c r="C43" s="43"/>
-      <c r="D43" s="28"/>
+      <c r="A43" t="s" s="33">
+        <v>254</v>
+      </c>
+      <c r="B43" t="s" s="35">
+        <v>212</v>
+      </c>
+      <c r="C43" t="s" s="33">
+        <v>21</v>
+      </c>
+      <c r="D43" s="39"/>
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
-      <c r="I43" s="28"/>
-      <c r="J43" s="28"/>
-    </row>
-    <row r="44" ht="15.25" customHeight="1">
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
+    </row>
+    <row r="44" ht="16" customHeight="1">
       <c r="A44" t="s" s="33">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="B44" t="s" s="35">
-        <v>184</v>
+        <v>256</v>
       </c>
       <c r="C44" t="s" s="33">
         <v>21</v>
@@ -12612,10 +12648,10 @@
     </row>
     <row r="45" ht="15.25" customHeight="1">
       <c r="A45" t="s" s="33">
-        <v>244</v>
+        <v>257</v>
       </c>
       <c r="B45" t="s" s="35">
-        <v>212</v>
+        <v>258</v>
       </c>
       <c r="C45" t="s" s="33">
         <v>21</v>
@@ -12627,42 +12663,6 @@
       <c r="H45" s="28"/>
       <c r="I45" s="39"/>
       <c r="J45" s="39"/>
-    </row>
-    <row r="46" ht="16" customHeight="1">
-      <c r="A46" t="s" s="33">
-        <v>245</v>
-      </c>
-      <c r="B46" t="s" s="35">
-        <v>246</v>
-      </c>
-      <c r="C46" t="s" s="33">
-        <v>21</v>
-      </c>
-      <c r="D46" s="39"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
-    </row>
-    <row r="47" ht="15.25" customHeight="1">
-      <c r="A47" t="s" s="33">
-        <v>247</v>
-      </c>
-      <c r="B47" t="s" s="35">
-        <v>248</v>
-      </c>
-      <c r="C47" t="s" s="33">
-        <v>21</v>
-      </c>
-      <c r="D47" s="39"/>
-      <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12793,13 +12793,13 @@
   <sheetData>
     <row r="1" ht="15.35" customHeight="1">
       <c r="A1" t="s" s="70">
-        <v>250</v>
+        <v>260</v>
       </c>
       <c r="B1" t="s" s="70">
-        <v>251</v>
+        <v>261</v>
       </c>
       <c r="C1" t="s" s="70">
-        <v>252</v>
+        <v>262</v>
       </c>
       <c r="D1" s="71"/>
       <c r="E1" s="71"/>
@@ -12808,7 +12808,7 @@
     </row>
     <row r="2" ht="15.35" customHeight="1">
       <c r="A2" t="s" s="70">
-        <v>253</v>
+        <v>263</v>
       </c>
       <c r="B2" s="72">
         <v>6</v>
@@ -12823,7 +12823,7 @@
     </row>
     <row r="3" ht="15.35" customHeight="1">
       <c r="A3" t="s" s="70">
-        <v>254</v>
+        <v>264</v>
       </c>
       <c r="B3" s="72">
         <v>4</v>
@@ -12838,7 +12838,7 @@
     </row>
     <row r="4" ht="15.35" customHeight="1">
       <c r="A4" t="s" s="70">
-        <v>255</v>
+        <v>265</v>
       </c>
       <c r="B4" s="72">
         <v>4</v>
@@ -12853,7 +12853,7 @@
     </row>
     <row r="5" ht="15.35" customHeight="1">
       <c r="A5" t="s" s="70">
-        <v>256</v>
+        <v>266</v>
       </c>
       <c r="B5" s="72">
         <v>3</v>
@@ -12868,7 +12868,7 @@
     </row>
     <row r="6" ht="15.35" customHeight="1">
       <c r="A6" t="s" s="70">
-        <v>257</v>
+        <v>267</v>
       </c>
       <c r="B6" s="72">
         <v>2</v>

</xml_diff>